<commit_message>
Sat Dec 21 06:50:05 AM CST 2024
</commit_message>
<xml_diff>
--- a/bosai/summary_51/summary.xlsx
+++ b/bosai/summary_51/summary.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView windowWidth="28800" windowHeight="11355"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$22</definedName>
   </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>项目部月报   __生信_ 部   本周工作完成情况</t>
   </si>
@@ -61,6 +62,66 @@
     <t>备注/遇到问题</t>
   </si>
   <si>
+    <t>BSTF241223</t>
+  </si>
+  <si>
+    <t>邓玲玲</t>
+  </si>
+  <si>
+    <t>生信评估</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>BSXG240327</t>
+  </si>
+  <si>
+    <t>陈立茂</t>
+  </si>
+  <si>
+    <t>补充分析</t>
+  </si>
+  <si>
+    <t>基于血小板RNA测序数据预测早期肺癌潜在生物标志物</t>
+  </si>
+  <si>
+    <t>修改内容</t>
+  </si>
+  <si>
+    <t>BSJF240734</t>
+  </si>
+  <si>
+    <t>林波</t>
+  </si>
+  <si>
+    <t>生信分析</t>
+  </si>
+  <si>
+    <t>清心莲子饮网络药理学分析</t>
+  </si>
+  <si>
+    <t>还需补充文字说明</t>
+  </si>
+  <si>
+    <t>BS.develop</t>
+  </si>
+  <si>
+    <t>模块开发</t>
+  </si>
+  <si>
+    <t>GEO 数据库快速调研</t>
+  </si>
+  <si>
+    <t>以 EDirect (Unix) 和 GEOquery (R)，实现以关键词搜索获取数据集、元数据，取得样本分组信息，检测是否有充足临床数据 (例如生存时间等)。</t>
+  </si>
+  <si>
+    <t>生信分析动态文档</t>
+  </si>
+  <si>
+    <t>基于 step 体系 (我在上一个公司时搭建的分析体系)，嵌入动态文档功能，包含方法说明，一般分析总结，图片、表格说明 (待完善) 。</t>
+  </si>
+  <si>
     <t>需协调与帮助：暂无</t>
   </si>
   <si>
@@ -68,6 +129,42 @@
   </si>
   <si>
     <t>项目部月报   __生信_ 部    下周工作安排</t>
+  </si>
+  <si>
+    <t>BSZD231122</t>
+  </si>
+  <si>
+    <t>杨立宇</t>
+  </si>
+  <si>
+    <t>分析优化</t>
+  </si>
+  <si>
+    <t>骨肉瘤</t>
+  </si>
+  <si>
+    <t>BSHQ240941</t>
+  </si>
+  <si>
+    <t>梁海东</t>
+  </si>
+  <si>
+    <t>BSCL241113</t>
+  </si>
+  <si>
+    <t>邓姝</t>
+  </si>
+  <si>
+    <t>BSCL231024</t>
+  </si>
+  <si>
+    <t>宋飞</t>
+  </si>
+  <si>
+    <t>BSHQ240813</t>
+  </si>
+  <si>
+    <t>王凯</t>
   </si>
   <si>
     <t>预计需协调与帮助：</t>
@@ -76,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -788,7 +885,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -820,9 +917,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="0" fontId="5" numFmtId="14" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1354,23 +1448,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="13.6222222222222" customWidth="1"/>
-    <col min="3" max="3" width="15.7481481481481" customWidth="1"/>
-    <col min="4" max="8" width="13.6222222222222" customWidth="1"/>
-    <col min="9" max="9" width="41.5037037037037" customWidth="1"/>
+    <col min="1" max="2" width="13.6190476190476" customWidth="1"/>
+    <col min="3" max="3" width="15.752380952381" customWidth="1"/>
+    <col min="4" max="8" width="13.6190476190476" customWidth="1"/>
+    <col min="9" max="9" width="41.5047619047619" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="22.5" r="1" spans="1:9">
+    <row r="1" ht="22.5" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1477,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="9"/>
     </row>
-    <row ht="18" r="2" spans="1:9">
+    <row r="2" ht="16.5" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1412,174 +1506,152 @@
         <v>9</v>
       </c>
     </row>
-    <row ht="17.25" r="3" spans="1:9">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>BSTF241223</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>邓玲玲</t>
-        </is>
-      </c>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>生信评估</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E3" s="11">
+    <row r="3" ht="16.5" spans="1:9">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6">
         <v>45638</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="6">
         <v>45639</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="6">
         <v>45642</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="6">
         <v>45642</v>
       </c>
-      <c r="I3" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row ht="17.25" r="4" spans="1:9">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>BSJF240734</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>林波</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
-        <is>
-          <t>生信分析</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="inlineStr">
-        <is>
-          <t>清心莲子饮网络药理学分析</t>
-        </is>
-      </c>
-      <c r="E4" s="11">
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" ht="71.25" spans="1:9">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6">
+        <v>45544</v>
+      </c>
+      <c r="F4" s="6">
+        <v>45611</v>
+      </c>
+      <c r="G4" s="6">
+        <v>45622</v>
+      </c>
+      <c r="H4" s="6">
+        <v>45622</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" ht="42.75" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6">
         <v>45630</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F5" s="6">
         <v>45646</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G5" s="6">
         <v>45643</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H5" s="6">
         <v>45643</v>
       </c>
-      <c r="I4" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row ht="17.25" r="5" spans="1:9">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>BS.develop</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>模块开发</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>生信分析动态文档</t>
-        </is>
-      </c>
-      <c r="E5" s="11">
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" ht="66" spans="1:9">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6">
+        <v>45636</v>
+      </c>
+      <c r="F6" s="6">
+        <v>45637</v>
+      </c>
+      <c r="G6" s="6">
+        <v>45637</v>
+      </c>
+      <c r="H6" s="6">
+        <v>45637</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" ht="66" spans="1:9">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6">
         <v>45642</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F7" s="6">
         <v>45644</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G7" s="6">
         <v>45644</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H7" s="6">
         <v>45644</v>
       </c>
-      <c r="I5" s="3" t="inlineStr">
-        <is>
-          <t>基于 step 体系 (我在上一个公司时搭建的分析体系)，嵌入动态文档功能，做了优化，包括方法说明，阶段性分析结果。现已撰写网络药理学 (BATMAN-TCM)、limma 差异分析、lasso、survival、enrichment、ferrDb、GeneCard、stringdb、TCGA 等分析或数据库的动态文档。持续更新中。</t>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="6" spans="1:9">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>BS.develop</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>模块开发</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>GEO 数据库快速调研</t>
-        </is>
-      </c>
-      <c r="E6" s="11">
-        <v>45636</v>
-      </c>
-      <c r="F6" s="11">
-        <v>45637</v>
-      </c>
-      <c r="G6" s="11">
-        <v>45637</v>
-      </c>
-      <c r="H6" s="11">
-        <v>45637</v>
-      </c>
-      <c r="I6" s="3" t="inlineStr">
-        <is>
-          <t>以 EDirect (Unix) 和 GEOquery (R)，实现以关键词搜索获取数据集、元数据，取得样本分组信息，检测是否有充足临床数据 (例如生存时间等)。</t>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="7" spans="1:9">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row customFormat="1" ht="17.25" r="8" spans="1:9">
+      <c r="I7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" ht="16.5" spans="1:9">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1590,7 +1662,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="3"/>
     </row>
-    <row customFormat="1" ht="17.25" r="9" spans="1:9">
+    <row r="9" customFormat="1" ht="16.5" spans="1:9">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1601,7 +1673,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="3"/>
     </row>
-    <row customFormat="1" ht="17.25" r="10" spans="1:9">
+    <row r="10" customFormat="1" ht="16.5" spans="1:9">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1614,7 +1686,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1627,7 +1699,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1638,9 +1710,9 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row ht="22.5" r="13" spans="1:9">
+    <row r="13" ht="22.5" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1651,7 +1723,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="9"/>
     </row>
-    <row ht="18" r="14" spans="1:9">
+    <row r="14" ht="16.5" spans="1:9">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1680,265 +1752,163 @@
         <v>9</v>
       </c>
     </row>
-    <row customFormat="1" ht="17.25" r="15" spans="1:9">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t>BSZD231122</t>
-        </is>
-      </c>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>杨立宇</t>
-        </is>
-      </c>
-      <c r="C15" s="4" t="inlineStr">
-        <is>
-          <t>分析优化</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="inlineStr">
-        <is>
-          <t>骨肉瘤</t>
-        </is>
-      </c>
-      <c r="E15" s="11">
+    <row r="15" customFormat="1" ht="16.5" spans="1:9">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="6">
         <v>45254</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="6">
         <v>45604</v>
       </c>
-      <c r="G15" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H15" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I15" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="16" spans="1:9">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>BSLL230309</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>王建澍</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>分析优化</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="inlineStr">
-        <is>
-          <t>MEK5/ERK5信号通路通过调控Nur77促进骨肉瘤细胞增殖、迁移和侵袭</t>
-        </is>
-      </c>
-      <c r="E16" s="11">
-        <v>45102</v>
-      </c>
-      <c r="F16" s="11">
-        <v>45616</v>
-      </c>
-      <c r="G16" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H16" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I16" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="17" spans="1:9">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>BSHQ240941</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
-        <is>
-          <t>梁海东</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>生信分析</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E17" s="11">
+      <c r="G15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" ht="16.5" spans="1:9">
+      <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="6">
         <v>45595</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F16" s="6">
         <v>45639</v>
       </c>
-      <c r="G17" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H17" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I17" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="18" spans="1:9">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>BSCL241113</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>邓姝</t>
-        </is>
-      </c>
-      <c r="C18" s="4" t="inlineStr">
-        <is>
-          <t>生信分析</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E18" s="11">
+      <c r="G16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" ht="16.5" spans="1:9">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="6">
         <v>45625</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F17" s="6">
         <v>45639</v>
       </c>
-      <c r="G18" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H18" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I18" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="19" spans="1:9">
-      <c r="A19" s="4" t="inlineStr">
-        <is>
-          <t>BSCL231024</t>
-        </is>
-      </c>
-      <c r="B19" s="4" t="inlineStr">
-        <is>
-          <t>宋飞</t>
-        </is>
-      </c>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>生信分析</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E19" s="11">
+      <c r="G17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" ht="16.5" spans="1:9">
+      <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="6">
         <v>45619</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F18" s="6">
         <v>45639</v>
       </c>
-      <c r="G19" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H19" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I19" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="20" spans="1:9">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>BSHQ240813</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>王凯</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr">
-        <is>
-          <t>生信分析</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E20" s="11">
+      <c r="G18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" ht="16.5" spans="1:9">
+      <c r="A19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="6">
         <v>45595</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F19" s="6">
         <v>45639</v>
       </c>
-      <c r="G20" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H20" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I20" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customFormat="1" ht="17.25" r="21" spans="1:9">
+      <c r="G19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" ht="16.5" spans="1:9">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" customFormat="1" ht="16.5" spans="1:9">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1949,29 +1919,18 @@
       <c r="H21" s="6"/>
       <c r="I21" s="3"/>
     </row>
-    <row customFormat="1" ht="17.25" r="22" spans="1:9">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row ht="28.5" r="23" spans="1:9">
-      <c r="A23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="10"/>
+    <row r="22" customFormat="1" ht="28.5" spans="1:9">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1981,5 +1940,6 @@
     <mergeCell ref="A13:I13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>